<commit_message>
9/16/2020 - End Q4
</commit_message>
<xml_diff>
--- a/CIS655/CIS655.xlsx
+++ b/CIS655/CIS655.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captain\Syracuse\Syracuse\CIS655\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7DAD10-4E61-4139-AF1D-C28D1D7D67CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB3D1AA-90FB-43FA-98CB-E7FE82E8F946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="587" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Live 1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
     <sheet name="Live 5" sheetId="9" r:id="rId10"/>
     <sheet name="Live 6" sheetId="10" r:id="rId11"/>
+    <sheet name="Live 8" sheetId="12" r:id="rId12"/>
+    <sheet name="Live 9" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="803">
   <si>
     <t>TRY TO FIND A PAPER ON MEMORY, DO NOT FOCUS ON CPU</t>
   </si>
@@ -2439,6 +2441,474 @@
   </si>
   <si>
     <t>EX</t>
+  </si>
+  <si>
+    <t>10-11 slides</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>Two final exams</t>
+  </si>
+  <si>
+    <t>each is 10%</t>
+  </si>
+  <si>
+    <t>one is standard/nice/easy</t>
+  </si>
+  <si>
+    <t>read and summarize</t>
+  </si>
+  <si>
+    <t>second will be similar to HW2 and HW4</t>
+  </si>
+  <si>
+    <t>Assigned most likely next week</t>
+  </si>
+  <si>
+    <t>Midterm review</t>
+  </si>
+  <si>
+    <t>s0 and s0: data dependecy</t>
+  </si>
+  <si>
+    <t>t0 and t0: name dependency</t>
+  </si>
+  <si>
+    <t>the add before the loop has an issue with beq in loop</t>
+  </si>
+  <si>
+    <t>need two stalls for beq</t>
+  </si>
+  <si>
+    <t>no need for stall at addi after lw (load word, not store word)</t>
+  </si>
+  <si>
+    <t>needs one stall</t>
+  </si>
+  <si>
+    <t>instruction 5 needs stall: it's from instruction 3 (lw)</t>
+  </si>
+  <si>
+    <t>even with forwarding unit, no stall cycles</t>
+  </si>
+  <si>
+    <t>principle of locality</t>
+  </si>
+  <si>
+    <t>each block has two words</t>
+  </si>
+  <si>
+    <t>need to show mapping</t>
+  </si>
+  <si>
+    <t>need to make copies of block (two words) not just single word</t>
+  </si>
+  <si>
+    <t>once cache is full, we use LRU</t>
+  </si>
+  <si>
+    <t>should add one layer of optimization</t>
+  </si>
+  <si>
+    <t>load load load/add add add/store store store</t>
+  </si>
+  <si>
+    <t>AMAT Inst and AMAT data</t>
+  </si>
+  <si>
+    <t>ILP</t>
+  </si>
+  <si>
+    <t>thread: process with its own instructions and data</t>
+  </si>
+  <si>
+    <t>each thread has all the state data</t>
+  </si>
+  <si>
+    <t>multithreading</t>
+  </si>
+  <si>
+    <t>processor must duplicate indpendent state for each thread</t>
+  </si>
+  <si>
+    <t>Corse-grained multithreading</t>
+  </si>
+  <si>
+    <t>only switch threads if there is a real need to switch</t>
+  </si>
+  <si>
+    <t>fine grained</t>
+  </si>
+  <si>
+    <t>just switch every nanosecond (or similar)</t>
+  </si>
+  <si>
+    <t>no need to a do a fast switch since it only occurs when there is a real issue (page fault)</t>
+  </si>
+  <si>
+    <t>Parallel Architecture</t>
+  </si>
+  <si>
+    <t>message passing</t>
+  </si>
+  <si>
+    <t>2. message passing</t>
+  </si>
+  <si>
+    <t>1. shared address space</t>
+  </si>
+  <si>
+    <t>shared address space</t>
+  </si>
+  <si>
+    <t>each process can have a shared address space that is seen/accessable by other processes</t>
+  </si>
+  <si>
+    <t>Shared space is physically in main memory and all procesors can access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memory controllers have to be designed to manage multiple </t>
+  </si>
+  <si>
+    <t>add synchronization via send and receive</t>
+  </si>
+  <si>
+    <t>point to point communication</t>
+  </si>
+  <si>
+    <t>Types of units</t>
+  </si>
+  <si>
+    <t>symmetric multiprocessors (SMP)</t>
+  </si>
+  <si>
+    <t>small number of cores, simple programming, uniform memory access</t>
+  </si>
+  <si>
+    <t>processes pay the same cost/time to access the memory</t>
+  </si>
+  <si>
+    <t>no inconsistencies, only one copy of the data</t>
+  </si>
+  <si>
+    <t>distributed</t>
+  </si>
+  <si>
+    <t>memory distributed among processors</t>
+  </si>
+  <si>
+    <t>may get inconsistent data</t>
+  </si>
+  <si>
+    <t>non-uniform memory access: process clsoe to memeory will take less time to access the memory</t>
+  </si>
+  <si>
+    <t>processors connected via direct (switched) and non-direct (multi-hop) interconnection networks</t>
+  </si>
+  <si>
+    <t>Cache coherence</t>
+  </si>
+  <si>
+    <t>snooping vs. directory based</t>
+  </si>
+  <si>
+    <t>MSI Model</t>
+  </si>
+  <si>
+    <t>block (not word)</t>
+  </si>
+  <si>
+    <t>every block has one label (state)</t>
+  </si>
+  <si>
+    <t>either M, S, or I</t>
+  </si>
+  <si>
+    <t>I: either you don't have it, or you have an old version</t>
+  </si>
+  <si>
+    <t>Modified shared invald</t>
+  </si>
+  <si>
+    <t>S: only read it/accessed it, didn't make it dirty OR you can share this block with other processors</t>
+  </si>
+  <si>
+    <t>M: modified/mine: I just changed its value, its dirty</t>
+  </si>
+  <si>
+    <t>forces an S to I</t>
+  </si>
+  <si>
+    <t>snooping</t>
+  </si>
+  <si>
+    <t>shared block</t>
+  </si>
+  <si>
+    <t>local read: still S</t>
+  </si>
+  <si>
+    <t>Now block is modified</t>
+  </si>
+  <si>
+    <t>I did a local read AFTER I modified</t>
+  </si>
+  <si>
+    <t>still mine, still M</t>
+  </si>
+  <si>
+    <t>Now block is just modified by me: still M</t>
+  </si>
+  <si>
+    <t>now, what if block was I for me</t>
+  </si>
+  <si>
+    <t>I do a local write: it becomes mine (M)</t>
+  </si>
+  <si>
+    <t>while I was snooping in the bus, someone wrote to it (made it dirty)</t>
+  </si>
+  <si>
+    <t>now it's invalid (I)</t>
+  </si>
+  <si>
+    <t>now it was mine, while I was snooping, found a read request (someone else just did a local read)</t>
+  </si>
+  <si>
+    <t>now two people have S (no longer mine, it's now S for me and S for other)</t>
+  </si>
+  <si>
+    <t>Now it was not mine, it was an I, and I did a local read:</t>
+  </si>
+  <si>
+    <t>goes to S (shared)</t>
+  </si>
+  <si>
+    <t>even if you're not sharing it, but you don't mind that it is S</t>
+  </si>
+  <si>
+    <t>now it was shared, and I'm snooping on the bus, and I found a write request</t>
+  </si>
+  <si>
+    <t>my copy is now I</t>
+  </si>
+  <si>
+    <t>two were sharing, and a third writes</t>
+  </si>
+  <si>
+    <t>the copies are I</t>
+  </si>
+  <si>
+    <t>now it was shared, snooping on the bus, and found a read request</t>
+  </si>
+  <si>
+    <t>still S</t>
+  </si>
+  <si>
+    <t>now it was shared, and I did a local write</t>
+  </si>
+  <si>
+    <t>mine is M</t>
+  </si>
+  <si>
+    <t>other S is now I</t>
+  </si>
+  <si>
+    <t>now it's invalid, and while snooping, I found write or read</t>
+  </si>
+  <si>
+    <t>now it stays as I</t>
+  </si>
+  <si>
+    <t>if others have a shared block and modify/read/write/etc, I don't care</t>
+  </si>
+  <si>
+    <t>Shared messages/network</t>
+  </si>
+  <si>
+    <t>Four major networking domains:</t>
+  </si>
+  <si>
+    <t>OCN: on-chip network</t>
+  </si>
+  <si>
+    <t>very small, ARM</t>
+  </si>
+  <si>
+    <t>system/storage area networks (SANs)</t>
+  </si>
+  <si>
+    <t>Local Area Network (LAN)</t>
+  </si>
+  <si>
+    <t>Wide area network (WAN)</t>
+  </si>
+  <si>
+    <t>interconnect autonomous computer systems, things like ethernet</t>
+  </si>
+  <si>
+    <t>systems distributed across the globe</t>
+  </si>
+  <si>
+    <t>multiple access network: cannot have a dedicated line to each user</t>
+  </si>
+  <si>
+    <t>Final exam posted</t>
+  </si>
+  <si>
+    <t>Takehome</t>
+  </si>
+  <si>
+    <t>no presentation in front of professor</t>
+  </si>
+  <si>
+    <t>do at at home and submit</t>
+  </si>
+  <si>
+    <t>Online:</t>
+  </si>
+  <si>
+    <t>going to present/defend in front of professor</t>
+  </si>
+  <si>
+    <t>Tuesday 9/15/2020 LIVE</t>
+  </si>
+  <si>
+    <t>10% of total grade</t>
+  </si>
+  <si>
+    <t>Saturday 9/12/2020 midnight (your time zone)</t>
+  </si>
+  <si>
+    <t>One single PDF</t>
+  </si>
+  <si>
+    <t>SUBMIT TO RIGHT PLACE</t>
+  </si>
+  <si>
+    <t>No programming</t>
+  </si>
+  <si>
+    <t>Just a proposal/essay/bullets</t>
+  </si>
+  <si>
+    <t>Application: can be virtual/fake, or practical. Doesn't matter</t>
+  </si>
+  <si>
+    <t>could be in the future</t>
+  </si>
+  <si>
+    <t>something like a calculator, embedded system (security system)</t>
+  </si>
+  <si>
+    <t>propose a name</t>
+  </si>
+  <si>
+    <t>internal hardware: alu, forwarding unit, registers, etc</t>
+  </si>
+  <si>
+    <t>In order to convince, the application has to make sense to the proposal</t>
+  </si>
+  <si>
+    <t>can't have a space shuttle with two registers</t>
+  </si>
+  <si>
+    <t>two bit registers can only have four registers (can't say two bits with 100 registers)</t>
+  </si>
+  <si>
+    <t>can say three registers each with 8 bits</t>
+  </si>
+  <si>
+    <t>Must explain WHY you chose what you chose</t>
+  </si>
+  <si>
+    <t>if support from interent, must reference/cite</t>
+  </si>
+  <si>
+    <t>REUSE ASSIGNMENT 2 if you want</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must defend, professor will ask questions, code must react </t>
+  </si>
+  <si>
+    <t>This is the officially reported final exam</t>
+  </si>
+  <si>
+    <t>PDF file including the code summary and screenshots of the output AND a zipped folder of the code</t>
+  </si>
+  <si>
+    <t>Any language you like</t>
+  </si>
+  <si>
+    <t>IF/ID/…</t>
+  </si>
+  <si>
+    <t>program will detect pipeline hazards</t>
+  </si>
+  <si>
+    <t>Accept a program (not just an instruction line!) written in MIPS</t>
+  </si>
+  <si>
+    <t>can read program anyway</t>
+  </si>
+  <si>
+    <t>Output needs to be printed (could be excel file, text file, console, etc.)</t>
+  </si>
+  <si>
+    <t>F-D-X-M-W</t>
+  </si>
+  <si>
+    <t>F-S-D-X-M-W</t>
+  </si>
+  <si>
+    <t>Three outputs needed</t>
+  </si>
+  <si>
+    <t>Add, subtract, load, store</t>
+  </si>
+  <si>
+    <t>input program is four lines or more</t>
+  </si>
+  <si>
+    <t>Challenge: professor will change the instructions</t>
+  </si>
+  <si>
+    <t>in the input program</t>
+  </si>
+  <si>
+    <t>can you make the r1 into r2? Can you make the load a store? Etc?</t>
+  </si>
+  <si>
+    <t>branch: extra credit</t>
+  </si>
+  <si>
+    <t>taken/not taken</t>
+  </si>
+  <si>
+    <t>prediction: super extra credit</t>
+  </si>
+  <si>
+    <t>Submit code/PDF before midngiht 9/12/2020 (Saturday), but can make some modifications in between</t>
+  </si>
+  <si>
+    <t>8 minutes for presentation next week</t>
+  </si>
+  <si>
+    <t>propose something?</t>
+  </si>
+  <si>
+    <t>demo?</t>
+  </si>
+  <si>
+    <t>is it your demo or you found online?</t>
+  </si>
+  <si>
+    <t>4 mins for presentation/4 mins demo</t>
+  </si>
+  <si>
+    <t>arrows from one stage to another, extra credit as well</t>
   </si>
 </sst>
 </file>
@@ -2625,7 +3095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2649,22 +3119,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2676,15 +3131,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3995,7 +4466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
@@ -4249,8 +4720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959F3DDE-A25C-494B-B02D-2CBB55C01AF8}">
   <dimension ref="B2:Z112"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4520,6 +4991,10 @@
     <row r="62" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>494</v>
+      </c>
+      <c r="L62">
+        <f>2^6</f>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="3:16" x14ac:dyDescent="0.25">
@@ -4853,7 +5328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150EA7EC-3B06-482B-8385-A9CA1140B417}">
   <dimension ref="A3:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
       <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
@@ -5305,6 +5780,878 @@
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
         <v>627</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBDF2FD-495D-48AA-8817-0752547087F2}">
+  <dimension ref="B3:F137"/>
+  <sheetViews>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="K113" sqref="K113"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>403</v>
+      </c>
+      <c r="E22" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>704</v>
+      </c>
+      <c r="F91" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E121" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="123" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="124" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="125" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="126" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E126" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="128" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E136" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>740</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81141513-B09C-4073-8433-A46A20A7DC97}">
+  <dimension ref="B3:E74"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="22" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="7" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="7" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="22" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="7" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="7" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -5615,8 +6962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C055D0AC-AF3F-4150-9570-0AB1070922E3}">
   <dimension ref="B3:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6015,8 +7362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8742F395-CBDF-4A24-BDFC-381F5A6BE4EB}">
   <dimension ref="A2:AE130"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="O109" sqref="O109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7357,7 +8704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74899A1D-49D4-4464-A7E2-C717614D337B}">
   <dimension ref="A3:W76"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -7881,8 +9228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C55210-7128-4BE8-B9D7-03681E8AD1B5}">
   <dimension ref="A3:V79"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="W43" sqref="W43"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="AA50" sqref="AA50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8468,510 +9815,510 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>628</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>629</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="19"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="18">
+      <c r="A2" s="20"/>
+      <c r="B2" s="15">
         <v>1</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="15">
         <v>2</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="27">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="19">
+      <c r="E2" s="28"/>
+      <c r="F2" s="27">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="19">
+      <c r="G2" s="28"/>
+      <c r="H2" s="27">
         <v>5</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="18">
+      <c r="I2" s="28"/>
+      <c r="J2" s="15">
         <v>6</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="15">
         <v>7</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="15">
         <v>8</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="15">
         <v>9</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="15">
         <v>10</v>
       </c>
-      <c r="O2" s="18">
+      <c r="O2" s="15">
         <v>11</v>
       </c>
-      <c r="P2" s="18">
+      <c r="P2" s="15">
         <v>12</v>
       </c>
-      <c r="Q2" s="18">
+      <c r="Q2" s="15">
         <v>13</v>
       </c>
-      <c r="R2" s="18">
+      <c r="R2" s="15">
         <v>14</v>
       </c>
-      <c r="S2" s="18">
+      <c r="S2" s="15">
         <v>15</v>
       </c>
-      <c r="T2" s="18">
+      <c r="T2" s="15">
         <v>16</v>
       </c>
-      <c r="U2" s="18">
+      <c r="U2" s="15">
         <v>17</v>
       </c>
-      <c r="V2" s="18">
+      <c r="V2" s="15">
         <v>18</v>
       </c>
-      <c r="W2" s="18">
+      <c r="W2" s="15">
         <v>19</v>
       </c>
-      <c r="X2" s="18">
+      <c r="X2" s="15">
         <v>20</v>
       </c>
-      <c r="Y2" s="18">
+      <c r="Y2" s="15">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>631</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="27" t="s">
         <v>633</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="27" t="s">
         <v>634</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
     </row>
     <row r="4" spans="1:31" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>635</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15" t="s">
         <v>631</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="19" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="18" t="s">
+      <c r="I4" s="28"/>
+      <c r="J4" s="15" t="s">
         <v>646</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="AE4" s="26" t="s">
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="AE4" s="20" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="20" t="s">
         <v>636</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="19" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="18" t="s">
+      <c r="I5" s="28"/>
+      <c r="J5" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="AE5" s="26" t="s">
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="AE5" s="20" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="AE6" s="26" t="s">
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="AE6" s="20" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>640</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="AE7" s="26" t="s">
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="AE7" s="20" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="20" t="s">
         <v>641</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="Q8" s="18" t="s">
+      <c r="Q8" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="R8" s="18" t="s">
+      <c r="R8" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="S8" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="AE8" s="26" t="s">
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="AE8" s="20" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="20" t="s">
         <v>642</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="R9" s="21" t="s">
+      <c r="R9" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="S9" s="18" t="s">
+      <c r="S9" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="T9" s="18" t="s">
+      <c r="T9" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="U9" s="18" t="s">
+      <c r="U9" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="V9" s="18" t="s">
+      <c r="V9" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="AE9" s="26" t="s">
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="AE9" s="20" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="20" t="s">
         <v>643</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="T10" s="18" t="s">
+      <c r="T10" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="U10" s="18" t="s">
+      <c r="U10" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="V10" s="18" t="s">
+      <c r="V10" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="W10" s="18" t="s">
+      <c r="W10" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="AE10" s="26" t="s">
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="AE10" s="20" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="20" t="s">
         <v>644</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="U11" s="18" t="s">
+      <c r="U11" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="V11" s="18" t="s">
+      <c r="V11" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="W11" s="18" t="s">
+      <c r="W11" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="X11" s="18" t="s">
+      <c r="X11" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="Y11" s="18"/>
-      <c r="AE11" s="26" t="s">
+      <c r="Y11" s="15"/>
+      <c r="AE11" s="20" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AE12" s="26" t="s">
+      <c r="AE12" s="20" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="18" t="s">
         <v>628</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="17" t="s">
         <v>629</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="27"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -8987,429 +10334,429 @@
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
       <c r="X15" s="14"/>
-      <c r="Y15" s="25"/>
+      <c r="Y15" s="19"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="18">
+      <c r="A16" s="20"/>
+      <c r="B16" s="15">
         <v>1</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="15">
         <v>2</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="27">
         <v>3</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="19">
+      <c r="E16" s="28"/>
+      <c r="F16" s="27">
         <v>4</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="19">
+      <c r="G16" s="28"/>
+      <c r="H16" s="27">
         <v>5</v>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="18">
+      <c r="I16" s="28"/>
+      <c r="J16" s="15">
         <v>6</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="15">
         <v>7</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="15">
         <v>8</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="15">
         <v>9</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="15">
         <v>10</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="15">
         <v>11</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P16" s="15">
         <v>12</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="Q16" s="15">
         <v>13</v>
       </c>
-      <c r="R16" s="18">
+      <c r="R16" s="15">
         <v>14</v>
       </c>
-      <c r="S16" s="18">
+      <c r="S16" s="15">
         <v>15</v>
       </c>
-      <c r="T16" s="18">
+      <c r="T16" s="15">
         <v>16</v>
       </c>
-      <c r="U16" s="18">
+      <c r="U16" s="15">
         <v>17</v>
       </c>
-      <c r="V16" s="18">
+      <c r="V16" s="15">
         <v>18</v>
       </c>
-      <c r="W16" s="18">
+      <c r="W16" s="15">
         <v>19</v>
       </c>
-      <c r="X16" s="18">
+      <c r="X16" s="15">
         <v>20</v>
       </c>
-      <c r="Y16" s="18">
+      <c r="Y16" s="15">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>631</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="27" t="s">
         <v>633</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19" t="s">
+      <c r="E17" s="28"/>
+      <c r="F17" s="27" t="s">
         <v>634</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19" t="s">
+      <c r="G17" s="28"/>
+      <c r="H17" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
     </row>
     <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>635</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15" t="s">
         <v>631</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19" t="s">
+      <c r="E18" s="28"/>
+      <c r="F18" s="27" t="s">
         <v>646</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="19" t="s">
+      <c r="G18" s="28"/>
+      <c r="H18" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="18" t="s">
+      <c r="I18" s="28"/>
+      <c r="J18" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
     </row>
     <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="20" t="s">
         <v>636</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="19" t="s">
+      <c r="E19" s="28"/>
+      <c r="F19" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="19" t="s">
+      <c r="G19" s="28"/>
+      <c r="H19" s="27" t="s">
         <v>646</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="18" t="s">
+      <c r="I19" s="28"/>
+      <c r="J19" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="18"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
     </row>
     <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="19" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="19" t="s">
+      <c r="G20" s="28"/>
+      <c r="H20" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="18" t="s">
+      <c r="I20" s="28"/>
+      <c r="J20" s="15" t="s">
         <v>646</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="L20" s="18" t="s">
+      <c r="L20" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
     </row>
     <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>640</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="19" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="18" t="s">
+      <c r="I21" s="28"/>
+      <c r="J21" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="L21" s="18" t="s">
+      <c r="L21" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="M21" s="18" t="s">
+      <c r="M21" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="18"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="20" t="s">
         <v>641</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="18" t="s">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="L22" s="18" t="s">
+      <c r="L22" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="N22" s="18" t="s">
+      <c r="N22" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
     </row>
     <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="20" t="s">
         <v>642</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="L23" s="21" t="s">
+      <c r="L23" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="M23" s="18" t="s">
+      <c r="M23" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="N23" s="18" t="s">
+      <c r="N23" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="O23" s="18" t="s">
+      <c r="O23" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="P23" s="18" t="s">
+      <c r="P23" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="20" t="s">
         <v>643</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="N24" s="18" t="s">
+      <c r="N24" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="O24" s="18" t="s">
+      <c r="O24" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="P24" s="18" t="s">
+      <c r="P24" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="Q24" s="18" t="s">
+      <c r="Q24" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="R24" s="21"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="18"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="20" t="s">
         <v>644</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18" t="s">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="O25" s="18" t="s">
+      <c r="O25" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="P25" s="18" t="s">
+      <c r="P25" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="Q25" s="18" t="s">
+      <c r="Q25" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="R25" s="18" t="s">
+      <c r="R25" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="18"/>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="18"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="67">

</xml_diff>